<commit_message>
modified the dataset and the code
</commit_message>
<xml_diff>
--- a/dataset.xlsx
+++ b/dataset.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="30720" windowHeight="13380" activeTab="2"/>
+    <workbookView windowWidth="30720" windowHeight="13380"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="stablize time" sheetId="2" r:id="rId1"/>
+    <sheet name="experiment" sheetId="1" r:id="rId2"/>
     <sheet name="AfterCoffee" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -29,13 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="15">
-  <si>
-    <t>Helena</t>
-  </si>
-  <si>
-    <t>Yufeng</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="14">
   <si>
     <t>observation</t>
   </si>
@@ -49,10 +43,16 @@
     <t>device</t>
   </si>
   <si>
-    <t>start time</t>
+    <t>average stabilize</t>
   </si>
   <si>
     <t>12p/s</t>
+  </si>
+  <si>
+    <t>Helena</t>
+  </si>
+  <si>
+    <t>Yufeng</t>
   </si>
   <si>
     <t>testID</t>
@@ -61,19 +61,16 @@
     <t>time</t>
   </si>
   <si>
-    <t>notification</t>
+    <t>Immediate</t>
   </si>
   <si>
-    <t>4 immdiate</t>
+    <t>After 10 minutes</t>
   </si>
   <si>
-    <t>5 10min</t>
+    <t>After 20 minutes</t>
   </si>
   <si>
-    <t>6 20min</t>
-  </si>
-  <si>
-    <t>7 30min</t>
+    <t>After 30 minutes</t>
   </si>
 </sst>
 </file>
@@ -1004,10 +1001,448 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I44"/>
+  <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A49" sqref="A46:A49"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="3"/>
+  <cols>
+    <col min="1" max="1" width="19.8888888888889" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="2:2">
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9">
+        <v>5</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>75</v>
+      </c>
+      <c r="D9">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10">
+        <v>5</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>75</v>
+      </c>
+      <c r="D10">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11">
+        <v>5</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11">
+        <v>74</v>
+      </c>
+      <c r="D11">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12">
+        <v>5</v>
+      </c>
+      <c r="B12">
+        <v>3</v>
+      </c>
+      <c r="C12">
+        <v>74</v>
+      </c>
+      <c r="D12">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13">
+        <v>5</v>
+      </c>
+      <c r="B13">
+        <v>4</v>
+      </c>
+      <c r="C13">
+        <v>74</v>
+      </c>
+      <c r="D13">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14">
+        <v>5</v>
+      </c>
+      <c r="B14">
+        <v>5</v>
+      </c>
+      <c r="C14">
+        <v>74</v>
+      </c>
+      <c r="D14">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15">
+        <v>5</v>
+      </c>
+      <c r="B15">
+        <v>6</v>
+      </c>
+      <c r="C15">
+        <v>74</v>
+      </c>
+      <c r="D15">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16">
+        <v>5</v>
+      </c>
+      <c r="B16">
+        <v>7</v>
+      </c>
+      <c r="C16">
+        <v>74</v>
+      </c>
+      <c r="D16">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17">
+        <v>5</v>
+      </c>
+      <c r="B17">
+        <v>8</v>
+      </c>
+      <c r="C17">
+        <v>74</v>
+      </c>
+      <c r="D17">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18">
+        <v>5</v>
+      </c>
+      <c r="B18">
+        <v>9</v>
+      </c>
+      <c r="C18">
+        <v>74</v>
+      </c>
+      <c r="D18">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19">
+        <v>5</v>
+      </c>
+      <c r="B19">
+        <v>10</v>
+      </c>
+      <c r="C19">
+        <v>74</v>
+      </c>
+      <c r="D19">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20">
+        <v>5</v>
+      </c>
+      <c r="B20">
+        <v>11</v>
+      </c>
+      <c r="C20">
+        <v>74</v>
+      </c>
+      <c r="D20">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21">
+        <v>5</v>
+      </c>
+      <c r="B21">
+        <v>12</v>
+      </c>
+      <c r="C21">
+        <v>74</v>
+      </c>
+      <c r="D21">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22">
+        <v>5</v>
+      </c>
+      <c r="B22">
+        <v>13</v>
+      </c>
+      <c r="C22">
+        <v>74</v>
+      </c>
+      <c r="D22">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23">
+        <v>5</v>
+      </c>
+      <c r="B23">
+        <v>14</v>
+      </c>
+      <c r="C23">
+        <v>74</v>
+      </c>
+      <c r="D23">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24">
+        <v>5</v>
+      </c>
+      <c r="B24">
+        <v>15</v>
+      </c>
+      <c r="C24">
+        <v>74</v>
+      </c>
+      <c r="D24">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25">
+        <v>5</v>
+      </c>
+      <c r="B25">
+        <v>16</v>
+      </c>
+      <c r="C25">
+        <v>74</v>
+      </c>
+      <c r="D25">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26">
+        <v>5</v>
+      </c>
+      <c r="B26">
+        <v>17</v>
+      </c>
+      <c r="C26">
+        <v>74</v>
+      </c>
+      <c r="D26">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27">
+        <v>5</v>
+      </c>
+      <c r="B27">
+        <v>18</v>
+      </c>
+      <c r="C27">
+        <v>74</v>
+      </c>
+      <c r="D27">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28">
+        <v>5</v>
+      </c>
+      <c r="B28">
+        <v>19</v>
+      </c>
+      <c r="C28">
+        <v>74</v>
+      </c>
+      <c r="D28">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29">
+        <v>5</v>
+      </c>
+      <c r="B29">
+        <v>20</v>
+      </c>
+      <c r="C29">
+        <v>74</v>
+      </c>
+      <c r="D29">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30">
+        <v>5</v>
+      </c>
+      <c r="B30">
+        <v>21</v>
+      </c>
+      <c r="C30">
+        <v>74</v>
+      </c>
+      <c r="D30">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31">
+        <v>5</v>
+      </c>
+      <c r="B31">
+        <v>22</v>
+      </c>
+      <c r="C31">
+        <v>74</v>
+      </c>
+      <c r="D31">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32">
+        <v>5</v>
+      </c>
+      <c r="B32">
+        <v>23</v>
+      </c>
+      <c r="C32">
+        <v>74</v>
+      </c>
+      <c r="D32">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33">
+        <v>5</v>
+      </c>
+      <c r="B33">
+        <v>24</v>
+      </c>
+      <c r="C33">
+        <v>74</v>
+      </c>
+      <c r="D33">
+        <v>75</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:I38"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -1019,90 +1454,193 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>0</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="B1"/>
       <c r="F1" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" t="s">
-        <v>5</v>
-      </c>
       <c r="F2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" t="s">
         <v>2</v>
       </c>
-      <c r="G2" t="s">
+      <c r="I2" t="s">
         <v>3</v>
       </c>
-      <c r="H2" t="s">
-        <v>4</v>
-      </c>
-      <c r="I2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
         <v>0</v>
       </c>
-      <c r="B3">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
+      <c r="C3">
+        <v>72</v>
+      </c>
+      <c r="D3">
+        <v>76</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>86</v>
+      </c>
+      <c r="I3">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B4">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
+        <v>10</v>
+      </c>
+      <c r="C4">
+        <v>74</v>
+      </c>
+      <c r="D4">
+        <v>80</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>10</v>
+      </c>
+      <c r="H4">
+        <v>89</v>
+      </c>
+      <c r="I4">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B5">
         <v>20</v>
       </c>
-    </row>
-    <row r="6" spans="1:2">
+      <c r="C5">
+        <v>75</v>
+      </c>
+      <c r="D5">
+        <v>79</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>20</v>
+      </c>
+      <c r="H5">
+        <v>91</v>
+      </c>
+      <c r="I5">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B6">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
+        <v>30</v>
+      </c>
+      <c r="C6">
+        <v>76</v>
+      </c>
+      <c r="D6">
+        <v>77</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>30</v>
+      </c>
+      <c r="H6">
+        <v>91</v>
+      </c>
+      <c r="I6">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B7">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8" t="s">
-        <v>6</v>
+        <v>40</v>
+      </c>
+      <c r="C7">
+        <v>75</v>
+      </c>
+      <c r="D7">
+        <v>74</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>40</v>
+      </c>
+      <c r="H7">
+        <v>88</v>
+      </c>
+      <c r="I7">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8">
+        <v>1</v>
       </c>
       <c r="B8">
-        <v>23</v>
-      </c>
-      <c r="F8" t="s">
-        <v>6</v>
+        <v>50</v>
+      </c>
+      <c r="C8">
+        <v>75</v>
+      </c>
+      <c r="D8">
+        <v>77</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
       </c>
       <c r="G8">
-        <v>23</v>
+        <v>50</v>
+      </c>
+      <c r="H8">
+        <v>88</v>
+      </c>
+      <c r="I8">
+        <v>115</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -1110,25 +1648,25 @@
         <v>1</v>
       </c>
       <c r="B9">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="C9">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="D9">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="F9">
         <v>1</v>
       </c>
       <c r="G9">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="H9">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="I9">
-        <v>101</v>
+        <v>92</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -1136,25 +1674,25 @@
         <v>1</v>
       </c>
       <c r="B10">
-        <v>10</v>
+        <v>70</v>
       </c>
       <c r="C10">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="D10">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="F10">
         <v>1</v>
       </c>
       <c r="G10">
-        <v>10</v>
+        <v>70</v>
       </c>
       <c r="H10">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="I10">
-        <v>94</v>
+        <v>107</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -1162,25 +1700,25 @@
         <v>1</v>
       </c>
       <c r="B11">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="C11">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="D11">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F11">
         <v>1</v>
       </c>
       <c r="G11">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="H11">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="I11">
-        <v>100</v>
+        <v>92</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -1188,25 +1726,25 @@
         <v>1</v>
       </c>
       <c r="B12">
-        <v>30</v>
+        <v>90</v>
       </c>
       <c r="C12">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D12">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="F12">
         <v>1</v>
       </c>
       <c r="G12">
-        <v>30</v>
+        <v>90</v>
       </c>
       <c r="H12">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="I12">
-        <v>91</v>
+        <v>85</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -1214,25 +1752,25 @@
         <v>1</v>
       </c>
       <c r="B13">
-        <v>40</v>
+        <v>100</v>
       </c>
       <c r="C13">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="D13">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="F13">
         <v>1</v>
       </c>
       <c r="G13">
-        <v>40</v>
+        <v>100</v>
       </c>
       <c r="H13">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="I13">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -1240,100 +1778,100 @@
         <v>1</v>
       </c>
       <c r="B14">
-        <v>50</v>
+        <v>110</v>
       </c>
       <c r="C14">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="D14">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="F14">
         <v>1</v>
       </c>
       <c r="G14">
-        <v>50</v>
+        <v>110</v>
       </c>
       <c r="H14">
         <v>88</v>
       </c>
       <c r="I14">
-        <v>115</v>
+        <v>82</v>
       </c>
     </row>
     <row r="15" spans="1:9">
       <c r="A15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B15">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="C15">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="D15">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="F15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G15">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="H15">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="I15">
-        <v>92</v>
+        <v>102</v>
       </c>
     </row>
     <row r="16" spans="1:9">
       <c r="A16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B16">
-        <v>70</v>
+        <v>10</v>
       </c>
       <c r="C16">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="D16">
+        <v>101</v>
+      </c>
+      <c r="F16">
+        <v>2</v>
+      </c>
+      <c r="G16">
+        <v>10</v>
+      </c>
+      <c r="H16">
+        <v>87</v>
+      </c>
+      <c r="I16">
         <v>90</v>
-      </c>
-      <c r="F16">
-        <v>1</v>
-      </c>
-      <c r="G16">
-        <v>70</v>
-      </c>
-      <c r="H16">
-        <v>86</v>
-      </c>
-      <c r="I16">
-        <v>107</v>
       </c>
     </row>
     <row r="17" spans="1:9">
       <c r="A17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B17">
-        <v>80</v>
+        <v>20</v>
       </c>
       <c r="C17">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D17">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="F17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G17">
-        <v>80</v>
+        <v>20</v>
       </c>
       <c r="H17">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="I17">
         <v>92</v>
@@ -1341,77 +1879,77 @@
     </row>
     <row r="18" spans="1:9">
       <c r="A18">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B18">
-        <v>90</v>
+        <v>30</v>
       </c>
       <c r="C18">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D18">
         <v>80</v>
       </c>
       <c r="F18">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G18">
-        <v>90</v>
+        <v>30</v>
       </c>
       <c r="H18">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="I18">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="19" spans="1:9">
       <c r="A19">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B19">
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="C19">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="D19">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F19">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G19">
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="H19">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="I19">
-        <v>89</v>
+        <v>83</v>
       </c>
     </row>
     <row r="20" spans="1:9">
       <c r="A20">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B20">
-        <v>110</v>
+        <v>50</v>
       </c>
       <c r="C20">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="D20">
-        <v>88</v>
+        <v>106</v>
       </c>
       <c r="F20">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G20">
-        <v>110</v>
+        <v>50</v>
       </c>
       <c r="H20">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="I20">
         <v>82</v>
@@ -1422,25 +1960,25 @@
         <v>2</v>
       </c>
       <c r="B21">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="C21">
         <v>73</v>
       </c>
       <c r="D21">
-        <v>72</v>
+        <v>133</v>
       </c>
       <c r="F21">
         <v>2</v>
       </c>
       <c r="G21">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="H21">
         <v>83</v>
       </c>
       <c r="I21">
-        <v>102</v>
+        <v>88</v>
       </c>
     </row>
     <row r="22" spans="1:9">
@@ -1448,25 +1986,25 @@
         <v>2</v>
       </c>
       <c r="B22">
-        <v>10</v>
+        <v>70</v>
       </c>
       <c r="C22">
         <v>74</v>
       </c>
       <c r="D22">
-        <v>101</v>
+        <v>81</v>
       </c>
       <c r="F22">
         <v>2</v>
       </c>
       <c r="G22">
-        <v>10</v>
+        <v>70</v>
       </c>
       <c r="H22">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="I22">
-        <v>90</v>
+        <v>83</v>
       </c>
     </row>
     <row r="23" spans="1:9">
@@ -1474,10 +2012,10 @@
         <v>2</v>
       </c>
       <c r="B23">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="C23">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D23">
         <v>82</v>
@@ -1486,13 +2024,13 @@
         <v>2</v>
       </c>
       <c r="G23">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="H23">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="I23">
-        <v>92</v>
+        <v>82</v>
       </c>
     </row>
     <row r="24" spans="1:9">
@@ -1500,25 +2038,25 @@
         <v>2</v>
       </c>
       <c r="B24">
-        <v>30</v>
+        <v>90</v>
       </c>
       <c r="C24">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D24">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="F24">
         <v>2</v>
       </c>
       <c r="G24">
-        <v>30</v>
+        <v>90</v>
       </c>
       <c r="H24">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I24">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="25" spans="1:9">
@@ -1526,25 +2064,25 @@
         <v>2</v>
       </c>
       <c r="B25">
-        <v>40</v>
+        <v>100</v>
       </c>
       <c r="C25">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D25">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="F25">
         <v>2</v>
       </c>
       <c r="G25">
-        <v>40</v>
+        <v>100</v>
       </c>
       <c r="H25">
         <v>83</v>
       </c>
       <c r="I25">
-        <v>83</v>
+        <v>88</v>
       </c>
     </row>
     <row r="26" spans="1:9">
@@ -1552,181 +2090,181 @@
         <v>2</v>
       </c>
       <c r="B26">
-        <v>50</v>
+        <v>110</v>
       </c>
       <c r="C26">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D26">
-        <v>106</v>
+        <v>77</v>
       </c>
       <c r="F26">
         <v>2</v>
       </c>
       <c r="G26">
-        <v>50</v>
+        <v>110</v>
       </c>
       <c r="H26">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I26">
-        <v>82</v>
+        <v>88</v>
       </c>
     </row>
     <row r="27" spans="1:9">
       <c r="A27">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B27">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="C27">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="D27">
-        <v>133</v>
+        <v>78</v>
       </c>
       <c r="F27">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G27">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="H27">
         <v>83</v>
       </c>
       <c r="I27">
-        <v>88</v>
+        <v>93</v>
       </c>
     </row>
     <row r="28" spans="1:9">
       <c r="A28">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B28">
-        <v>70</v>
+        <v>10</v>
       </c>
       <c r="C28">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D28">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="F28">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G28">
-        <v>70</v>
+        <v>10</v>
       </c>
       <c r="H28">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="I28">
-        <v>83</v>
+        <v>97</v>
       </c>
     </row>
     <row r="29" spans="1:9">
       <c r="A29">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B29">
-        <v>80</v>
+        <v>20</v>
       </c>
       <c r="C29">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D29">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="F29">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G29">
-        <v>80</v>
+        <v>20</v>
       </c>
       <c r="H29">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="I29">
-        <v>82</v>
+        <v>132</v>
       </c>
     </row>
     <row r="30" spans="1:9">
       <c r="A30">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B30">
-        <v>90</v>
+        <v>30</v>
       </c>
       <c r="C30">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D30">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F30">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G30">
-        <v>90</v>
+        <v>30</v>
       </c>
       <c r="H30">
+        <v>84</v>
+      </c>
+      <c r="I30">
         <v>81</v>
-      </c>
-      <c r="I30">
-        <v>83</v>
       </c>
     </row>
     <row r="31" spans="1:9">
       <c r="A31">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B31">
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="C31">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D31">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="F31">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G31">
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="H31">
         <v>83</v>
       </c>
       <c r="I31">
-        <v>88</v>
+        <v>80</v>
       </c>
     </row>
     <row r="32" spans="1:9">
       <c r="A32">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B32">
-        <v>110</v>
+        <v>50</v>
       </c>
       <c r="C32">
         <v>74</v>
       </c>
       <c r="D32">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="F32">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G32">
-        <v>110</v>
+        <v>50</v>
       </c>
       <c r="H32">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="I32">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="33" spans="1:9">
@@ -1734,25 +2272,25 @@
         <v>3</v>
       </c>
       <c r="B33">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="C33">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="D33">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="F33">
         <v>3</v>
       </c>
       <c r="G33">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="H33">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="I33">
-        <v>93</v>
+        <v>102</v>
       </c>
     </row>
     <row r="34" spans="1:9">
@@ -1760,25 +2298,25 @@
         <v>3</v>
       </c>
       <c r="B34">
-        <v>10</v>
+        <v>70</v>
       </c>
       <c r="C34">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D34">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="F34">
         <v>3</v>
       </c>
       <c r="G34">
-        <v>10</v>
+        <v>70</v>
       </c>
       <c r="H34">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="I34">
-        <v>97</v>
+        <v>85</v>
       </c>
     </row>
     <row r="35" spans="1:9">
@@ -1786,25 +2324,25 @@
         <v>3</v>
       </c>
       <c r="B35">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="C35">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D35">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="F35">
         <v>3</v>
       </c>
       <c r="G35">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="H35">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="I35">
-        <v>132</v>
+        <v>93</v>
       </c>
     </row>
     <row r="36" spans="1:9">
@@ -1812,25 +2350,25 @@
         <v>3</v>
       </c>
       <c r="B36">
-        <v>30</v>
+        <v>90</v>
       </c>
       <c r="C36">
         <v>73</v>
       </c>
       <c r="D36">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="F36">
         <v>3</v>
       </c>
       <c r="G36">
-        <v>30</v>
+        <v>90</v>
       </c>
       <c r="H36">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="I36">
-        <v>81</v>
+        <v>101</v>
       </c>
     </row>
     <row r="37" spans="1:9">
@@ -1838,25 +2376,25 @@
         <v>3</v>
       </c>
       <c r="B37">
-        <v>40</v>
+        <v>100</v>
       </c>
       <c r="C37">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D37">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F37">
         <v>3</v>
       </c>
       <c r="G37">
-        <v>40</v>
+        <v>100</v>
       </c>
       <c r="H37">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="I37">
-        <v>80</v>
+        <v>98</v>
       </c>
     </row>
     <row r="38" spans="1:9">
@@ -1864,10 +2402,10 @@
         <v>3</v>
       </c>
       <c r="B38">
-        <v>50</v>
+        <v>110</v>
       </c>
       <c r="C38">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D38">
         <v>79</v>
@@ -1876,538 +2414,13 @@
         <v>3</v>
       </c>
       <c r="G38">
-        <v>50</v>
+        <v>110</v>
       </c>
       <c r="H38">
-        <v>79</v>
+        <v>89</v>
       </c>
       <c r="I38">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9">
-      <c r="A39">
-        <v>3</v>
-      </c>
-      <c r="B39">
-        <v>60</v>
-      </c>
-      <c r="C39">
-        <v>73</v>
-      </c>
-      <c r="D39">
-        <v>81</v>
-      </c>
-      <c r="F39">
-        <v>3</v>
-      </c>
-      <c r="G39">
-        <v>60</v>
-      </c>
-      <c r="H39">
-        <v>81</v>
-      </c>
-      <c r="I39">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9">
-      <c r="A40">
-        <v>3</v>
-      </c>
-      <c r="B40">
-        <v>70</v>
-      </c>
-      <c r="C40">
-        <v>76</v>
-      </c>
-      <c r="D40">
-        <v>82</v>
-      </c>
-      <c r="F40">
-        <v>3</v>
-      </c>
-      <c r="G40">
-        <v>70</v>
-      </c>
-      <c r="H40">
-        <v>86</v>
-      </c>
-      <c r="I40">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9">
-      <c r="A41">
-        <v>3</v>
-      </c>
-      <c r="B41">
-        <v>80</v>
-      </c>
-      <c r="C41">
-        <v>73</v>
-      </c>
-      <c r="D41">
-        <v>74</v>
-      </c>
-      <c r="F41">
-        <v>3</v>
-      </c>
-      <c r="G41">
-        <v>80</v>
-      </c>
-      <c r="H41">
-        <v>87</v>
-      </c>
-      <c r="I41">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9">
-      <c r="A42">
-        <v>3</v>
-      </c>
-      <c r="B42">
-        <v>90</v>
-      </c>
-      <c r="C42">
-        <v>73</v>
-      </c>
-      <c r="D42">
-        <v>77</v>
-      </c>
-      <c r="F42">
-        <v>3</v>
-      </c>
-      <c r="G42">
-        <v>90</v>
-      </c>
-      <c r="H42">
-        <v>88</v>
-      </c>
-      <c r="I42">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9">
-      <c r="A43">
-        <v>3</v>
-      </c>
-      <c r="B43">
-        <v>100</v>
-      </c>
-      <c r="C43">
-        <v>75</v>
-      </c>
-      <c r="D43">
-        <v>75</v>
-      </c>
-      <c r="F43">
-        <v>3</v>
-      </c>
-      <c r="G43">
-        <v>100</v>
-      </c>
-      <c r="H43">
-        <v>90</v>
-      </c>
-      <c r="I43">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9">
-      <c r="A44">
-        <v>3</v>
-      </c>
-      <c r="B44">
-        <v>110</v>
-      </c>
-      <c r="C44">
-        <v>73</v>
-      </c>
-      <c r="D44">
-        <v>79</v>
-      </c>
-      <c r="F44">
-        <v>3</v>
-      </c>
-      <c r="G44">
-        <v>110</v>
-      </c>
-      <c r="H44">
-        <v>89</v>
-      </c>
-      <c r="I44">
         <v>84</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:D33"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="3"/>
-  <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3">
-        <v>0</v>
-      </c>
-      <c r="B3">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4">
-        <v>0</v>
-      </c>
-      <c r="B4">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5">
-        <v>0</v>
-      </c>
-      <c r="B5">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6">
-        <v>0</v>
-      </c>
-      <c r="B6">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="2:2">
-      <c r="B8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9">
-        <v>1</v>
-      </c>
-      <c r="B9">
-        <v>0</v>
-      </c>
-      <c r="C9">
-        <v>75</v>
-      </c>
-      <c r="D9">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10">
-        <v>1</v>
-      </c>
-      <c r="B10">
-        <v>1</v>
-      </c>
-      <c r="C10">
-        <v>75</v>
-      </c>
-      <c r="D10">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11">
-        <v>1</v>
-      </c>
-      <c r="B11">
-        <v>2</v>
-      </c>
-      <c r="C11">
-        <v>74</v>
-      </c>
-      <c r="D11">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="12" spans="2:4">
-      <c r="B12">
-        <v>3</v>
-      </c>
-      <c r="C12">
-        <v>74</v>
-      </c>
-      <c r="D12">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="13" spans="2:4">
-      <c r="B13">
-        <v>4</v>
-      </c>
-      <c r="C13">
-        <v>74</v>
-      </c>
-      <c r="D13">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="14" spans="2:4">
-      <c r="B14">
-        <v>5</v>
-      </c>
-      <c r="C14">
-        <v>74</v>
-      </c>
-      <c r="D14">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="15" spans="2:4">
-      <c r="B15">
-        <v>6</v>
-      </c>
-      <c r="C15">
-        <v>74</v>
-      </c>
-      <c r="D15">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="16" spans="2:4">
-      <c r="B16">
-        <v>7</v>
-      </c>
-      <c r="C16">
-        <v>74</v>
-      </c>
-      <c r="D16">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4">
-      <c r="B17">
-        <v>8</v>
-      </c>
-      <c r="C17">
-        <v>74</v>
-      </c>
-      <c r="D17">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4">
-      <c r="B18">
-        <v>9</v>
-      </c>
-      <c r="C18">
-        <v>74</v>
-      </c>
-      <c r="D18">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4">
-      <c r="B19">
-        <v>10</v>
-      </c>
-      <c r="C19">
-        <v>74</v>
-      </c>
-      <c r="D19">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="20" spans="2:4">
-      <c r="B20">
-        <v>11</v>
-      </c>
-      <c r="C20">
-        <v>74</v>
-      </c>
-      <c r="D20">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4">
-      <c r="B21">
-        <v>12</v>
-      </c>
-      <c r="C21">
-        <v>74</v>
-      </c>
-      <c r="D21">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="22" spans="2:4">
-      <c r="B22">
-        <v>13</v>
-      </c>
-      <c r="C22">
-        <v>74</v>
-      </c>
-      <c r="D22">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="23" spans="2:4">
-      <c r="B23">
-        <v>14</v>
-      </c>
-      <c r="C23">
-        <v>74</v>
-      </c>
-      <c r="D23">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="24" spans="2:4">
-      <c r="B24">
-        <v>15</v>
-      </c>
-      <c r="C24">
-        <v>74</v>
-      </c>
-      <c r="D24">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="25" spans="2:4">
-      <c r="B25">
-        <v>16</v>
-      </c>
-      <c r="C25">
-        <v>74</v>
-      </c>
-      <c r="D25">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="26" spans="2:4">
-      <c r="B26">
-        <v>17</v>
-      </c>
-      <c r="C26">
-        <v>74</v>
-      </c>
-      <c r="D26">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="27" spans="2:4">
-      <c r="B27">
-        <v>18</v>
-      </c>
-      <c r="C27">
-        <v>74</v>
-      </c>
-      <c r="D27">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="28" spans="2:4">
-      <c r="B28">
-        <v>19</v>
-      </c>
-      <c r="C28">
-        <v>74</v>
-      </c>
-      <c r="D28">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="29" spans="2:4">
-      <c r="B29">
-        <v>20</v>
-      </c>
-      <c r="C29">
-        <v>74</v>
-      </c>
-      <c r="D29">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="30" spans="2:4">
-      <c r="B30">
-        <v>21</v>
-      </c>
-      <c r="C30">
-        <v>74</v>
-      </c>
-      <c r="D30">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="31" spans="2:4">
-      <c r="B31">
-        <v>22</v>
-      </c>
-      <c r="C31">
-        <v>74</v>
-      </c>
-      <c r="D31">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="32" spans="2:4">
-      <c r="B32">
-        <v>23</v>
-      </c>
-      <c r="C32">
-        <v>74</v>
-      </c>
-      <c r="D32">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="33" spans="2:4">
-      <c r="B33">
-        <v>24</v>
-      </c>
-      <c r="C33">
-        <v>74</v>
-      </c>
-      <c r="D33">
-        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -2420,15 +2433,18 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E49"/>
+  <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="3"/>
+  <cols>
+    <col min="1" max="1" width="19.8888888888889" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -2436,18 +2452,15 @@
         <v>9</v>
       </c>
       <c r="C1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2">
-        <v>4</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -2458,13 +2471,10 @@
       <c r="D2">
         <v>75</v>
       </c>
-      <c r="E2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3">
-        <v>4</v>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>10</v>
       </c>
       <c r="B3">
         <v>10</v>
@@ -2475,13 +2485,10 @@
       <c r="D3">
         <v>77</v>
       </c>
-      <c r="E3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4">
-        <v>4</v>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>10</v>
       </c>
       <c r="B4">
         <v>20</v>
@@ -2492,13 +2499,10 @@
       <c r="D4">
         <v>68</v>
       </c>
-      <c r="E4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5">
-        <v>4</v>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>10</v>
       </c>
       <c r="B5">
         <v>30</v>
@@ -2509,13 +2513,10 @@
       <c r="D5">
         <v>83</v>
       </c>
-      <c r="E5" t="s">
-        <v>14</v>
-      </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6">
-        <v>4</v>
+      <c r="A6" t="s">
+        <v>10</v>
       </c>
       <c r="B6">
         <v>40</v>
@@ -2528,8 +2529,8 @@
       </c>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7">
-        <v>4</v>
+      <c r="A7" t="s">
+        <v>10</v>
       </c>
       <c r="B7">
         <v>50</v>
@@ -2542,8 +2543,8 @@
       </c>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8">
-        <v>4</v>
+      <c r="A8" t="s">
+        <v>10</v>
       </c>
       <c r="B8">
         <v>60</v>
@@ -2556,8 +2557,8 @@
       </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9">
-        <v>4</v>
+      <c r="A9" t="s">
+        <v>10</v>
       </c>
       <c r="B9">
         <v>70</v>
@@ -2570,8 +2571,8 @@
       </c>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10">
-        <v>4</v>
+      <c r="A10" t="s">
+        <v>10</v>
       </c>
       <c r="B10">
         <v>80</v>
@@ -2584,8 +2585,8 @@
       </c>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11">
-        <v>4</v>
+      <c r="A11" t="s">
+        <v>10</v>
       </c>
       <c r="B11">
         <v>90</v>
@@ -2598,8 +2599,8 @@
       </c>
     </row>
     <row r="12" spans="1:4">
-      <c r="A12">
-        <v>4</v>
+      <c r="A12" t="s">
+        <v>10</v>
       </c>
       <c r="B12">
         <v>100</v>
@@ -2612,8 +2613,8 @@
       </c>
     </row>
     <row r="13" spans="1:4">
-      <c r="A13">
-        <v>4</v>
+      <c r="A13" t="s">
+        <v>10</v>
       </c>
       <c r="B13">
         <v>110</v>
@@ -2626,8 +2627,8 @@
       </c>
     </row>
     <row r="14" spans="1:4">
-      <c r="A14">
-        <v>5</v>
+      <c r="A14" t="s">
+        <v>11</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -2640,8 +2641,8 @@
       </c>
     </row>
     <row r="15" spans="1:4">
-      <c r="A15">
-        <v>5</v>
+      <c r="A15" t="s">
+        <v>11</v>
       </c>
       <c r="B15">
         <v>10</v>
@@ -2654,8 +2655,8 @@
       </c>
     </row>
     <row r="16" spans="1:4">
-      <c r="A16">
-        <v>5</v>
+      <c r="A16" t="s">
+        <v>11</v>
       </c>
       <c r="B16">
         <v>20</v>
@@ -2668,8 +2669,8 @@
       </c>
     </row>
     <row r="17" spans="1:4">
-      <c r="A17">
-        <v>5</v>
+      <c r="A17" t="s">
+        <v>11</v>
       </c>
       <c r="B17">
         <v>30</v>
@@ -2682,8 +2683,8 @@
       </c>
     </row>
     <row r="18" spans="1:4">
-      <c r="A18">
-        <v>5</v>
+      <c r="A18" t="s">
+        <v>11</v>
       </c>
       <c r="B18">
         <v>40</v>
@@ -2696,8 +2697,8 @@
       </c>
     </row>
     <row r="19" spans="1:4">
-      <c r="A19">
-        <v>5</v>
+      <c r="A19" t="s">
+        <v>11</v>
       </c>
       <c r="B19">
         <v>50</v>
@@ -2710,8 +2711,8 @@
       </c>
     </row>
     <row r="20" spans="1:4">
-      <c r="A20">
-        <v>5</v>
+      <c r="A20" t="s">
+        <v>11</v>
       </c>
       <c r="B20">
         <v>60</v>
@@ -2724,8 +2725,8 @@
       </c>
     </row>
     <row r="21" spans="1:4">
-      <c r="A21">
-        <v>5</v>
+      <c r="A21" t="s">
+        <v>11</v>
       </c>
       <c r="B21">
         <v>70</v>
@@ -2738,8 +2739,8 @@
       </c>
     </row>
     <row r="22" spans="1:4">
-      <c r="A22">
-        <v>5</v>
+      <c r="A22" t="s">
+        <v>11</v>
       </c>
       <c r="B22">
         <v>80</v>
@@ -2752,8 +2753,8 @@
       </c>
     </row>
     <row r="23" spans="1:4">
-      <c r="A23">
-        <v>5</v>
+      <c r="A23" t="s">
+        <v>11</v>
       </c>
       <c r="B23">
         <v>90</v>
@@ -2766,8 +2767,8 @@
       </c>
     </row>
     <row r="24" spans="1:4">
-      <c r="A24">
-        <v>5</v>
+      <c r="A24" t="s">
+        <v>11</v>
       </c>
       <c r="B24">
         <v>100</v>
@@ -2780,8 +2781,8 @@
       </c>
     </row>
     <row r="25" spans="1:4">
-      <c r="A25">
-        <v>5</v>
+      <c r="A25" t="s">
+        <v>11</v>
       </c>
       <c r="B25">
         <v>110</v>
@@ -2794,8 +2795,8 @@
       </c>
     </row>
     <row r="26" spans="1:4">
-      <c r="A26">
-        <v>6</v>
+      <c r="A26" t="s">
+        <v>12</v>
       </c>
       <c r="B26">
         <v>0</v>
@@ -2808,8 +2809,8 @@
       </c>
     </row>
     <row r="27" spans="1:4">
-      <c r="A27">
-        <v>6</v>
+      <c r="A27" t="s">
+        <v>12</v>
       </c>
       <c r="B27">
         <v>10</v>
@@ -2822,8 +2823,8 @@
       </c>
     </row>
     <row r="28" spans="1:4">
-      <c r="A28">
-        <v>6</v>
+      <c r="A28" t="s">
+        <v>12</v>
       </c>
       <c r="B28">
         <v>20</v>
@@ -2836,8 +2837,8 @@
       </c>
     </row>
     <row r="29" spans="1:4">
-      <c r="A29">
-        <v>6</v>
+      <c r="A29" t="s">
+        <v>12</v>
       </c>
       <c r="B29">
         <v>30</v>
@@ -2850,8 +2851,8 @@
       </c>
     </row>
     <row r="30" spans="1:4">
-      <c r="A30">
-        <v>6</v>
+      <c r="A30" t="s">
+        <v>12</v>
       </c>
       <c r="B30">
         <v>40</v>
@@ -2864,8 +2865,8 @@
       </c>
     </row>
     <row r="31" spans="1:4">
-      <c r="A31">
-        <v>6</v>
+      <c r="A31" t="s">
+        <v>12</v>
       </c>
       <c r="B31">
         <v>50</v>
@@ -2878,8 +2879,8 @@
       </c>
     </row>
     <row r="32" spans="1:4">
-      <c r="A32">
-        <v>6</v>
+      <c r="A32" t="s">
+        <v>12</v>
       </c>
       <c r="B32">
         <v>60</v>
@@ -2892,8 +2893,8 @@
       </c>
     </row>
     <row r="33" spans="1:4">
-      <c r="A33">
-        <v>6</v>
+      <c r="A33" t="s">
+        <v>12</v>
       </c>
       <c r="B33">
         <v>70</v>
@@ -2906,8 +2907,8 @@
       </c>
     </row>
     <row r="34" spans="1:4">
-      <c r="A34">
-        <v>6</v>
+      <c r="A34" t="s">
+        <v>12</v>
       </c>
       <c r="B34">
         <v>80</v>
@@ -2920,8 +2921,8 @@
       </c>
     </row>
     <row r="35" spans="1:4">
-      <c r="A35">
-        <v>6</v>
+      <c r="A35" t="s">
+        <v>12</v>
       </c>
       <c r="B35">
         <v>90</v>
@@ -2934,8 +2935,8 @@
       </c>
     </row>
     <row r="36" spans="1:4">
-      <c r="A36">
-        <v>6</v>
+      <c r="A36" t="s">
+        <v>12</v>
       </c>
       <c r="B36">
         <v>100</v>
@@ -2948,8 +2949,8 @@
       </c>
     </row>
     <row r="37" spans="1:4">
-      <c r="A37">
-        <v>6</v>
+      <c r="A37" t="s">
+        <v>12</v>
       </c>
       <c r="B37">
         <v>110</v>
@@ -2962,8 +2963,8 @@
       </c>
     </row>
     <row r="38" spans="1:4">
-      <c r="A38">
-        <v>7</v>
+      <c r="A38" t="s">
+        <v>13</v>
       </c>
       <c r="B38">
         <v>0</v>
@@ -2976,8 +2977,8 @@
       </c>
     </row>
     <row r="39" spans="1:4">
-      <c r="A39">
-        <v>7</v>
+      <c r="A39" t="s">
+        <v>13</v>
       </c>
       <c r="B39">
         <v>10</v>
@@ -2990,8 +2991,8 @@
       </c>
     </row>
     <row r="40" spans="1:4">
-      <c r="A40">
-        <v>7</v>
+      <c r="A40" t="s">
+        <v>13</v>
       </c>
       <c r="B40">
         <v>20</v>
@@ -3004,8 +3005,8 @@
       </c>
     </row>
     <row r="41" spans="1:4">
-      <c r="A41">
-        <v>7</v>
+      <c r="A41" t="s">
+        <v>13</v>
       </c>
       <c r="B41">
         <v>30</v>
@@ -3018,8 +3019,8 @@
       </c>
     </row>
     <row r="42" spans="1:4">
-      <c r="A42">
-        <v>7</v>
+      <c r="A42" t="s">
+        <v>13</v>
       </c>
       <c r="B42">
         <v>40</v>
@@ -3032,8 +3033,8 @@
       </c>
     </row>
     <row r="43" spans="1:4">
-      <c r="A43">
-        <v>7</v>
+      <c r="A43" t="s">
+        <v>13</v>
       </c>
       <c r="B43">
         <v>50</v>
@@ -3046,8 +3047,8 @@
       </c>
     </row>
     <row r="44" spans="1:4">
-      <c r="A44">
-        <v>7</v>
+      <c r="A44" t="s">
+        <v>13</v>
       </c>
       <c r="B44">
         <v>60</v>
@@ -3060,8 +3061,8 @@
       </c>
     </row>
     <row r="45" spans="1:4">
-      <c r="A45">
-        <v>7</v>
+      <c r="A45" t="s">
+        <v>13</v>
       </c>
       <c r="B45">
         <v>70</v>
@@ -3074,8 +3075,8 @@
       </c>
     </row>
     <row r="46" spans="1:4">
-      <c r="A46">
-        <v>7</v>
+      <c r="A46" t="s">
+        <v>13</v>
       </c>
       <c r="B46">
         <v>80</v>
@@ -3088,8 +3089,8 @@
       </c>
     </row>
     <row r="47" spans="1:4">
-      <c r="A47">
-        <v>7</v>
+      <c r="A47" t="s">
+        <v>13</v>
       </c>
       <c r="B47">
         <v>90</v>
@@ -3102,8 +3103,8 @@
       </c>
     </row>
     <row r="48" spans="1:4">
-      <c r="A48">
-        <v>7</v>
+      <c r="A48" t="s">
+        <v>13</v>
       </c>
       <c r="B48">
         <v>100</v>
@@ -3116,8 +3117,8 @@
       </c>
     </row>
     <row r="49" spans="1:4">
-      <c r="A49">
-        <v>7</v>
+      <c r="A49" t="s">
+        <v>13</v>
       </c>
       <c r="B49">
         <v>110</v>

</xml_diff>

<commit_message>
add a Bland-Altman test
</commit_message>
<xml_diff>
--- a/dataset.xlsx
+++ b/dataset.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="30720" windowHeight="13380"/>
+    <workbookView windowWidth="30720" windowHeight="13380" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="stablize time" sheetId="2" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="12">
   <si>
     <t>observation</t>
   </si>
@@ -47,12 +47,6 @@
   </si>
   <si>
     <t>12p/s</t>
-  </si>
-  <si>
-    <t>Helena</t>
-  </si>
-  <si>
-    <t>Yufeng</t>
   </si>
   <si>
     <t>testID</t>
@@ -1003,7 +997,7 @@
   <sheetPr/>
   <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
@@ -1439,987 +1433,1038 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I38"/>
+  <dimension ref="A1:D73"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="3"/>
   <cols>
     <col min="1" max="1" width="12.2685185185185" customWidth="1"/>
     <col min="5" max="5" width="12.3611111111111" customWidth="1"/>
     <col min="6" max="6" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1"/>
-      <c r="F1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
-      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="F2" t="s">
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
         <v>0</v>
       </c>
-      <c r="G2" t="s">
-        <v>1</v>
-      </c>
-      <c r="H2" t="s">
-        <v>2</v>
-      </c>
-      <c r="I2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
+      <c r="C2">
+        <v>72</v>
+      </c>
+      <c r="D2">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C3">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D3">
-        <v>76</v>
-      </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-      <c r="H3">
-        <v>86</v>
-      </c>
-      <c r="I3">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4">
         <v>1</v>
       </c>
       <c r="B4">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C4">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D4">
-        <v>80</v>
-      </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-      <c r="G4">
-        <v>10</v>
-      </c>
-      <c r="H4">
-        <v>89</v>
-      </c>
-      <c r="I4">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5">
         <v>1</v>
       </c>
       <c r="B5">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C5">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D5">
-        <v>79</v>
-      </c>
-      <c r="F5">
-        <v>1</v>
-      </c>
-      <c r="G5">
-        <v>20</v>
-      </c>
-      <c r="H5">
-        <v>91</v>
-      </c>
-      <c r="I5">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6">
         <v>1</v>
       </c>
       <c r="B6">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="C6">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D6">
-        <v>77</v>
-      </c>
-      <c r="F6">
-        <v>1</v>
-      </c>
-      <c r="G6">
-        <v>30</v>
-      </c>
-      <c r="H6">
-        <v>91</v>
-      </c>
-      <c r="I6">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7">
         <v>1</v>
       </c>
       <c r="B7">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="C7">
         <v>75</v>
       </c>
       <c r="D7">
-        <v>74</v>
-      </c>
-      <c r="F7">
-        <v>1</v>
-      </c>
-      <c r="G7">
-        <v>40</v>
-      </c>
-      <c r="H7">
-        <v>88</v>
-      </c>
-      <c r="I7">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8">
         <v>1</v>
       </c>
       <c r="B8">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="C8">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="D8">
         <v>77</v>
       </c>
-      <c r="F8">
-        <v>1</v>
-      </c>
-      <c r="G8">
-        <v>50</v>
-      </c>
-      <c r="H8">
-        <v>88</v>
-      </c>
-      <c r="I8">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9">
         <v>1</v>
       </c>
       <c r="B9">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="C9">
         <v>78</v>
       </c>
       <c r="D9">
-        <v>77</v>
-      </c>
-      <c r="F9">
-        <v>1</v>
-      </c>
-      <c r="G9">
-        <v>60</v>
-      </c>
-      <c r="H9">
         <v>90</v>
       </c>
-      <c r="I9">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10">
         <v>1</v>
       </c>
       <c r="B10">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="C10">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="D10">
-        <v>90</v>
-      </c>
-      <c r="F10">
-        <v>1</v>
-      </c>
-      <c r="G10">
-        <v>70</v>
-      </c>
-      <c r="H10">
-        <v>86</v>
-      </c>
-      <c r="I10">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11">
         <v>1</v>
       </c>
       <c r="B11">
+        <v>90</v>
+      </c>
+      <c r="C11">
+        <v>77</v>
+      </c>
+      <c r="D11">
         <v>80</v>
       </c>
-      <c r="C11">
-        <v>80</v>
-      </c>
-      <c r="D11">
-        <v>77</v>
-      </c>
-      <c r="F11">
-        <v>1</v>
-      </c>
-      <c r="G11">
-        <v>80</v>
-      </c>
-      <c r="H11">
-        <v>88</v>
-      </c>
-      <c r="I11">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9">
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12">
         <v>1</v>
       </c>
       <c r="B12">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="C12">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D12">
         <v>80</v>
       </c>
-      <c r="F12">
-        <v>1</v>
-      </c>
-      <c r="G12">
-        <v>90</v>
-      </c>
-      <c r="H12">
-        <v>86</v>
-      </c>
-      <c r="I12">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
+    </row>
+    <row r="13" spans="1:4">
       <c r="A13">
         <v>1</v>
       </c>
       <c r="B13">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="C13">
         <v>78</v>
       </c>
       <c r="D13">
-        <v>80</v>
-      </c>
-      <c r="F13">
-        <v>1</v>
-      </c>
-      <c r="G13">
-        <v>100</v>
-      </c>
-      <c r="H13">
-        <v>85</v>
-      </c>
-      <c r="I13">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
       <c r="A14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B14">
-        <v>110</v>
+        <v>0</v>
       </c>
       <c r="C14">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="D14">
-        <v>88</v>
-      </c>
-      <c r="F14">
-        <v>1</v>
-      </c>
-      <c r="G14">
-        <v>110</v>
-      </c>
-      <c r="H14">
-        <v>88</v>
-      </c>
-      <c r="I14">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
       <c r="A15">
         <v>2</v>
       </c>
       <c r="B15">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C15">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D15">
-        <v>72</v>
-      </c>
-      <c r="F15">
-        <v>2</v>
-      </c>
-      <c r="G15">
-        <v>0</v>
-      </c>
-      <c r="H15">
-        <v>83</v>
-      </c>
-      <c r="I15">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
       <c r="A16">
         <v>2</v>
       </c>
       <c r="B16">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C16">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="D16">
-        <v>101</v>
-      </c>
-      <c r="F16">
-        <v>2</v>
-      </c>
-      <c r="G16">
-        <v>10</v>
-      </c>
-      <c r="H16">
-        <v>87</v>
-      </c>
-      <c r="I16">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
       <c r="A17">
         <v>2</v>
       </c>
       <c r="B17">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C17">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D17">
-        <v>82</v>
-      </c>
-      <c r="F17">
-        <v>2</v>
-      </c>
-      <c r="G17">
-        <v>20</v>
-      </c>
-      <c r="H17">
-        <v>86</v>
-      </c>
-      <c r="I17">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
       <c r="A18">
         <v>2</v>
       </c>
       <c r="B18">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="C18">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="D18">
-        <v>80</v>
-      </c>
-      <c r="F18">
-        <v>2</v>
-      </c>
-      <c r="G18">
-        <v>30</v>
-      </c>
-      <c r="H18">
-        <v>82</v>
-      </c>
-      <c r="I18">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
       <c r="A19">
         <v>2</v>
       </c>
       <c r="B19">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="C19">
         <v>72</v>
       </c>
       <c r="D19">
-        <v>75</v>
-      </c>
-      <c r="F19">
-        <v>2</v>
-      </c>
-      <c r="G19">
-        <v>40</v>
-      </c>
-      <c r="H19">
-        <v>83</v>
-      </c>
-      <c r="I19">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
       <c r="A20">
         <v>2</v>
       </c>
       <c r="B20">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="C20">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D20">
-        <v>106</v>
-      </c>
-      <c r="F20">
-        <v>2</v>
-      </c>
-      <c r="G20">
-        <v>50</v>
-      </c>
-      <c r="H20">
-        <v>86</v>
-      </c>
-      <c r="I20">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
       <c r="A21">
         <v>2</v>
       </c>
       <c r="B21">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="C21">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D21">
-        <v>133</v>
-      </c>
-      <c r="F21">
-        <v>2</v>
-      </c>
-      <c r="G21">
-        <v>60</v>
-      </c>
-      <c r="H21">
-        <v>83</v>
-      </c>
-      <c r="I21">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
       <c r="A22">
         <v>2</v>
       </c>
       <c r="B22">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="C22">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D22">
-        <v>81</v>
-      </c>
-      <c r="F22">
-        <v>2</v>
-      </c>
-      <c r="G22">
-        <v>70</v>
-      </c>
-      <c r="H22">
-        <v>85</v>
-      </c>
-      <c r="I22">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
       <c r="A23">
         <v>2</v>
       </c>
       <c r="B23">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="C23">
         <v>75</v>
       </c>
       <c r="D23">
-        <v>82</v>
-      </c>
-      <c r="F23">
-        <v>2</v>
-      </c>
-      <c r="G23">
-        <v>80</v>
-      </c>
-      <c r="H23">
-        <v>82</v>
-      </c>
-      <c r="I23">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
       <c r="A24">
         <v>2</v>
       </c>
       <c r="B24">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="C24">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D24">
-        <v>76</v>
-      </c>
-      <c r="F24">
-        <v>2</v>
-      </c>
-      <c r="G24">
-        <v>90</v>
-      </c>
-      <c r="H24">
         <v>81</v>
       </c>
-      <c r="I24">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9">
+    </row>
+    <row r="25" spans="1:4">
       <c r="A25">
         <v>2</v>
       </c>
       <c r="B25">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="C25">
         <v>74</v>
       </c>
       <c r="D25">
-        <v>81</v>
-      </c>
-      <c r="F25">
-        <v>2</v>
-      </c>
-      <c r="G25">
-        <v>100</v>
-      </c>
-      <c r="H25">
-        <v>83</v>
-      </c>
-      <c r="I25">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
       <c r="A26">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B26">
-        <v>110</v>
+        <v>0</v>
       </c>
       <c r="C26">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="D26">
-        <v>77</v>
-      </c>
-      <c r="F26">
-        <v>2</v>
-      </c>
-      <c r="G26">
-        <v>110</v>
-      </c>
-      <c r="H26">
-        <v>85</v>
-      </c>
-      <c r="I26">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
       <c r="A27">
         <v>3</v>
       </c>
       <c r="B27">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C27">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D27">
-        <v>78</v>
-      </c>
-      <c r="F27">
-        <v>3</v>
-      </c>
-      <c r="G27">
-        <v>0</v>
-      </c>
-      <c r="H27">
-        <v>83</v>
-      </c>
-      <c r="I27">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
       <c r="A28">
         <v>3</v>
       </c>
       <c r="B28">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C28">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D28">
-        <v>75</v>
-      </c>
-      <c r="F28">
-        <v>3</v>
-      </c>
-      <c r="G28">
-        <v>10</v>
-      </c>
-      <c r="H28">
-        <v>83</v>
-      </c>
-      <c r="I28">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
       <c r="A29">
         <v>3</v>
       </c>
       <c r="B29">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C29">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D29">
-        <v>72</v>
-      </c>
-      <c r="F29">
-        <v>3</v>
-      </c>
-      <c r="G29">
-        <v>20</v>
-      </c>
-      <c r="H29">
-        <v>83</v>
-      </c>
-      <c r="I29">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
       <c r="A30">
         <v>3</v>
       </c>
       <c r="B30">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="C30">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D30">
-        <v>73</v>
-      </c>
-      <c r="F30">
-        <v>3</v>
-      </c>
-      <c r="G30">
-        <v>30</v>
-      </c>
-      <c r="H30">
-        <v>84</v>
-      </c>
-      <c r="I30">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
       <c r="A31">
         <v>3</v>
       </c>
       <c r="B31">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="C31">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D31">
-        <v>76</v>
-      </c>
-      <c r="F31">
-        <v>3</v>
-      </c>
-      <c r="G31">
-        <v>40</v>
-      </c>
-      <c r="H31">
-        <v>83</v>
-      </c>
-      <c r="I31">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
       <c r="A32">
         <v>3</v>
       </c>
       <c r="B32">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="C32">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D32">
-        <v>79</v>
-      </c>
-      <c r="F32">
-        <v>3</v>
-      </c>
-      <c r="G32">
-        <v>50</v>
-      </c>
-      <c r="H32">
-        <v>79</v>
-      </c>
-      <c r="I32">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
       <c r="A33">
         <v>3</v>
       </c>
       <c r="B33">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="C33">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="D33">
-        <v>81</v>
-      </c>
-      <c r="F33">
-        <v>3</v>
-      </c>
-      <c r="G33">
-        <v>60</v>
-      </c>
-      <c r="H33">
-        <v>81</v>
-      </c>
-      <c r="I33">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
       <c r="A34">
         <v>3</v>
       </c>
       <c r="B34">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="C34">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D34">
-        <v>82</v>
-      </c>
-      <c r="F34">
-        <v>3</v>
-      </c>
-      <c r="G34">
-        <v>70</v>
-      </c>
-      <c r="H34">
-        <v>86</v>
-      </c>
-      <c r="I34">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
       <c r="A35">
         <v>3</v>
       </c>
       <c r="B35">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="C35">
         <v>73</v>
       </c>
       <c r="D35">
-        <v>74</v>
-      </c>
-      <c r="F35">
-        <v>3</v>
-      </c>
-      <c r="G35">
-        <v>80</v>
-      </c>
-      <c r="H35">
-        <v>87</v>
-      </c>
-      <c r="I35">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
       <c r="A36">
         <v>3</v>
       </c>
       <c r="B36">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="C36">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="D36">
-        <v>77</v>
-      </c>
-      <c r="F36">
-        <v>3</v>
-      </c>
-      <c r="G36">
-        <v>90</v>
-      </c>
-      <c r="H36">
-        <v>88</v>
-      </c>
-      <c r="I36">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
       <c r="A37">
         <v>3</v>
       </c>
       <c r="B37">
+        <v>110</v>
+      </c>
+      <c r="C37">
+        <v>73</v>
+      </c>
+      <c r="D37">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38">
+        <v>4</v>
+      </c>
+      <c r="B38">
+        <v>0</v>
+      </c>
+      <c r="C38">
+        <v>86</v>
+      </c>
+      <c r="D38">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39">
+        <v>4</v>
+      </c>
+      <c r="B39">
+        <v>10</v>
+      </c>
+      <c r="C39">
+        <v>89</v>
+      </c>
+      <c r="D39">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40">
+        <v>4</v>
+      </c>
+      <c r="B40">
+        <v>20</v>
+      </c>
+      <c r="C40">
+        <v>91</v>
+      </c>
+      <c r="D40">
         <v>100</v>
       </c>
-      <c r="C37">
-        <v>75</v>
-      </c>
-      <c r="D37">
-        <v>75</v>
-      </c>
-      <c r="F37">
-        <v>3</v>
-      </c>
-      <c r="G37">
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41">
+        <v>4</v>
+      </c>
+      <c r="B41">
+        <v>30</v>
+      </c>
+      <c r="C41">
+        <v>91</v>
+      </c>
+      <c r="D41">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42">
+        <v>4</v>
+      </c>
+      <c r="B42">
+        <v>40</v>
+      </c>
+      <c r="C42">
+        <v>88</v>
+      </c>
+      <c r="D42">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43">
+        <v>4</v>
+      </c>
+      <c r="B43">
+        <v>50</v>
+      </c>
+      <c r="C43">
+        <v>88</v>
+      </c>
+      <c r="D43">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44">
+        <v>4</v>
+      </c>
+      <c r="B44">
+        <v>60</v>
+      </c>
+      <c r="C44">
+        <v>90</v>
+      </c>
+      <c r="D44">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45">
+        <v>4</v>
+      </c>
+      <c r="B45">
+        <v>70</v>
+      </c>
+      <c r="C45">
+        <v>86</v>
+      </c>
+      <c r="D45">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46">
+        <v>4</v>
+      </c>
+      <c r="B46">
+        <v>80</v>
+      </c>
+      <c r="C46">
+        <v>88</v>
+      </c>
+      <c r="D46">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47">
+        <v>4</v>
+      </c>
+      <c r="B47">
+        <v>90</v>
+      </c>
+      <c r="C47">
+        <v>86</v>
+      </c>
+      <c r="D47">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48">
+        <v>4</v>
+      </c>
+      <c r="B48">
         <v>100</v>
       </c>
-      <c r="H37">
+      <c r="C48">
+        <v>85</v>
+      </c>
+      <c r="D48">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49">
+        <v>4</v>
+      </c>
+      <c r="B49">
+        <v>110</v>
+      </c>
+      <c r="C49">
+        <v>88</v>
+      </c>
+      <c r="D49">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50">
+        <v>5</v>
+      </c>
+      <c r="B50">
+        <v>0</v>
+      </c>
+      <c r="C50">
+        <v>83</v>
+      </c>
+      <c r="D50">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
+      <c r="A51">
+        <v>5</v>
+      </c>
+      <c r="B51">
+        <v>10</v>
+      </c>
+      <c r="C51">
+        <v>87</v>
+      </c>
+      <c r="D51">
         <v>90</v>
       </c>
-      <c r="I37">
+    </row>
+    <row r="52" spans="1:4">
+      <c r="A52">
+        <v>5</v>
+      </c>
+      <c r="B52">
+        <v>20</v>
+      </c>
+      <c r="C52">
+        <v>86</v>
+      </c>
+      <c r="D52">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
+      <c r="A53">
+        <v>5</v>
+      </c>
+      <c r="B53">
+        <v>30</v>
+      </c>
+      <c r="C53">
+        <v>82</v>
+      </c>
+      <c r="D53">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
+      <c r="A54">
+        <v>5</v>
+      </c>
+      <c r="B54">
+        <v>40</v>
+      </c>
+      <c r="C54">
+        <v>83</v>
+      </c>
+      <c r="D54">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
+      <c r="A55">
+        <v>5</v>
+      </c>
+      <c r="B55">
+        <v>50</v>
+      </c>
+      <c r="C55">
+        <v>86</v>
+      </c>
+      <c r="D55">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
+      <c r="A56">
+        <v>5</v>
+      </c>
+      <c r="B56">
+        <v>60</v>
+      </c>
+      <c r="C56">
+        <v>83</v>
+      </c>
+      <c r="D56">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4">
+      <c r="A57">
+        <v>5</v>
+      </c>
+      <c r="B57">
+        <v>70</v>
+      </c>
+      <c r="C57">
+        <v>85</v>
+      </c>
+      <c r="D57">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
+      <c r="A58">
+        <v>5</v>
+      </c>
+      <c r="B58">
+        <v>80</v>
+      </c>
+      <c r="C58">
+        <v>82</v>
+      </c>
+      <c r="D58">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
+      <c r="A59">
+        <v>5</v>
+      </c>
+      <c r="B59">
+        <v>90</v>
+      </c>
+      <c r="C59">
+        <v>81</v>
+      </c>
+      <c r="D59">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
+      <c r="A60">
+        <v>5</v>
+      </c>
+      <c r="B60">
+        <v>100</v>
+      </c>
+      <c r="C60">
+        <v>83</v>
+      </c>
+      <c r="D60">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4">
+      <c r="A61">
+        <v>5</v>
+      </c>
+      <c r="B61">
+        <v>110</v>
+      </c>
+      <c r="C61">
+        <v>85</v>
+      </c>
+      <c r="D61">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4">
+      <c r="A62">
+        <v>6</v>
+      </c>
+      <c r="B62">
+        <v>0</v>
+      </c>
+      <c r="C62">
+        <v>83</v>
+      </c>
+      <c r="D62">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4">
+      <c r="A63">
+        <v>6</v>
+      </c>
+      <c r="B63">
+        <v>10</v>
+      </c>
+      <c r="C63">
+        <v>83</v>
+      </c>
+      <c r="D63">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4">
+      <c r="A64">
+        <v>6</v>
+      </c>
+      <c r="B64">
+        <v>20</v>
+      </c>
+      <c r="C64">
+        <v>83</v>
+      </c>
+      <c r="D64">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4">
+      <c r="A65">
+        <v>6</v>
+      </c>
+      <c r="B65">
+        <v>30</v>
+      </c>
+      <c r="C65">
+        <v>84</v>
+      </c>
+      <c r="D65">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4">
+      <c r="A66">
+        <v>6</v>
+      </c>
+      <c r="B66">
+        <v>40</v>
+      </c>
+      <c r="C66">
+        <v>83</v>
+      </c>
+      <c r="D66">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4">
+      <c r="A67">
+        <v>6</v>
+      </c>
+      <c r="B67">
+        <v>50</v>
+      </c>
+      <c r="C67">
+        <v>79</v>
+      </c>
+      <c r="D67">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4">
+      <c r="A68">
+        <v>6</v>
+      </c>
+      <c r="B68">
+        <v>60</v>
+      </c>
+      <c r="C68">
+        <v>81</v>
+      </c>
+      <c r="D68">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4">
+      <c r="A69">
+        <v>6</v>
+      </c>
+      <c r="B69">
+        <v>70</v>
+      </c>
+      <c r="C69">
+        <v>86</v>
+      </c>
+      <c r="D69">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4">
+      <c r="A70">
+        <v>6</v>
+      </c>
+      <c r="B70">
+        <v>80</v>
+      </c>
+      <c r="C70">
+        <v>87</v>
+      </c>
+      <c r="D70">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4">
+      <c r="A71">
+        <v>6</v>
+      </c>
+      <c r="B71">
+        <v>90</v>
+      </c>
+      <c r="C71">
+        <v>88</v>
+      </c>
+      <c r="D71">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4">
+      <c r="A72">
+        <v>6</v>
+      </c>
+      <c r="B72">
+        <v>100</v>
+      </c>
+      <c r="C72">
+        <v>90</v>
+      </c>
+      <c r="D72">
         <v>98</v>
       </c>
     </row>
-    <row r="38" spans="1:9">
-      <c r="A38">
-        <v>3</v>
-      </c>
-      <c r="B38">
+    <row r="73" spans="1:4">
+      <c r="A73">
+        <v>6</v>
+      </c>
+      <c r="B73">
         <v>110</v>
       </c>
-      <c r="C38">
-        <v>73</v>
-      </c>
-      <c r="D38">
-        <v>79</v>
-      </c>
-      <c r="F38">
-        <v>3</v>
-      </c>
-      <c r="G38">
-        <v>110</v>
-      </c>
-      <c r="H38">
+      <c r="C73">
         <v>89</v>
       </c>
-      <c r="I38">
+      <c r="D73">
         <v>84</v>
       </c>
     </row>
@@ -2446,10 +2491,10 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -2460,7 +2505,7 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -2474,7 +2519,7 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B3">
         <v>10</v>
@@ -2488,7 +2533,7 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B4">
         <v>20</v>
@@ -2502,7 +2547,7 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B5">
         <v>30</v>
@@ -2516,7 +2561,7 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B6">
         <v>40</v>
@@ -2530,7 +2575,7 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B7">
         <v>50</v>
@@ -2544,7 +2589,7 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B8">
         <v>60</v>
@@ -2558,7 +2603,7 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B9">
         <v>70</v>
@@ -2572,7 +2617,7 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B10">
         <v>80</v>
@@ -2586,7 +2631,7 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B11">
         <v>90</v>
@@ -2600,7 +2645,7 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B12">
         <v>100</v>
@@ -2614,7 +2659,7 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B13">
         <v>110</v>
@@ -2628,7 +2673,7 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -2642,7 +2687,7 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B15">
         <v>10</v>
@@ -2656,7 +2701,7 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B16">
         <v>20</v>
@@ -2670,7 +2715,7 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B17">
         <v>30</v>
@@ -2684,7 +2729,7 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B18">
         <v>40</v>
@@ -2698,7 +2743,7 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B19">
         <v>50</v>
@@ -2712,7 +2757,7 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B20">
         <v>60</v>
@@ -2726,7 +2771,7 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B21">
         <v>70</v>
@@ -2740,7 +2785,7 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B22">
         <v>80</v>
@@ -2754,7 +2799,7 @@
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B23">
         <v>90</v>
@@ -2768,7 +2813,7 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B24">
         <v>100</v>
@@ -2782,7 +2827,7 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B25">
         <v>110</v>
@@ -2796,7 +2841,7 @@
     </row>
     <row r="26" spans="1:4">
       <c r="A26" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B26">
         <v>0</v>
@@ -2810,7 +2855,7 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B27">
         <v>10</v>
@@ -2824,7 +2869,7 @@
     </row>
     <row r="28" spans="1:4">
       <c r="A28" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B28">
         <v>20</v>
@@ -2838,7 +2883,7 @@
     </row>
     <row r="29" spans="1:4">
       <c r="A29" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B29">
         <v>30</v>
@@ -2852,7 +2897,7 @@
     </row>
     <row r="30" spans="1:4">
       <c r="A30" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B30">
         <v>40</v>
@@ -2866,7 +2911,7 @@
     </row>
     <row r="31" spans="1:4">
       <c r="A31" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B31">
         <v>50</v>
@@ -2880,7 +2925,7 @@
     </row>
     <row r="32" spans="1:4">
       <c r="A32" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B32">
         <v>60</v>
@@ -2894,7 +2939,7 @@
     </row>
     <row r="33" spans="1:4">
       <c r="A33" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B33">
         <v>70</v>
@@ -2908,7 +2953,7 @@
     </row>
     <row r="34" spans="1:4">
       <c r="A34" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B34">
         <v>80</v>
@@ -2922,7 +2967,7 @@
     </row>
     <row r="35" spans="1:4">
       <c r="A35" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B35">
         <v>90</v>
@@ -2936,7 +2981,7 @@
     </row>
     <row r="36" spans="1:4">
       <c r="A36" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B36">
         <v>100</v>
@@ -2950,7 +2995,7 @@
     </row>
     <row r="37" spans="1:4">
       <c r="A37" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B37">
         <v>110</v>
@@ -2964,7 +3009,7 @@
     </row>
     <row r="38" spans="1:4">
       <c r="A38" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B38">
         <v>0</v>
@@ -2978,7 +3023,7 @@
     </row>
     <row r="39" spans="1:4">
       <c r="A39" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B39">
         <v>10</v>
@@ -2992,7 +3037,7 @@
     </row>
     <row r="40" spans="1:4">
       <c r="A40" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B40">
         <v>20</v>
@@ -3006,7 +3051,7 @@
     </row>
     <row r="41" spans="1:4">
       <c r="A41" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B41">
         <v>30</v>
@@ -3020,7 +3065,7 @@
     </row>
     <row r="42" spans="1:4">
       <c r="A42" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B42">
         <v>40</v>
@@ -3034,7 +3079,7 @@
     </row>
     <row r="43" spans="1:4">
       <c r="A43" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B43">
         <v>50</v>
@@ -3048,7 +3093,7 @@
     </row>
     <row r="44" spans="1:4">
       <c r="A44" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B44">
         <v>60</v>
@@ -3062,7 +3107,7 @@
     </row>
     <row r="45" spans="1:4">
       <c r="A45" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B45">
         <v>70</v>
@@ -3076,7 +3121,7 @@
     </row>
     <row r="46" spans="1:4">
       <c r="A46" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B46">
         <v>80</v>
@@ -3090,7 +3135,7 @@
     </row>
     <row r="47" spans="1:4">
       <c r="A47" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B47">
         <v>90</v>
@@ -3104,7 +3149,7 @@
     </row>
     <row r="48" spans="1:4">
       <c r="A48" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B48">
         <v>100</v>
@@ -3118,7 +3163,7 @@
     </row>
     <row r="49" spans="1:4">
       <c r="A49" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B49">
         <v>110</v>

</xml_diff>